<commit_message>
Add excel get list functionality
</commit_message>
<xml_diff>
--- a/Grades 2021 Fall/CSC 440 2021 Fall.xlsx
+++ b/Grades 2021 Fall/CSC 440 2021 Fall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micah\Desktop\CSC440SoloProject\Grades 2021 Fall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CA62A8-FD41-4465-9B6F-92CBD88D36F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E5982C-8028-4660-9742-AD7334F3322A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29895" yWindow="1995" windowWidth="21600" windowHeight="11385" xr2:uid="{94745F47-4085-4EBA-B027-DBA26C8D34E0}"/>
   </bookViews>
@@ -34,48 +34,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
-  <si>
-    <t>StudentID</t>
-  </si>
-  <si>
-    <t>CoursePrefix</t>
-  </si>
-  <si>
-    <t>CourseNum</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Grade</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Semester</t>
-  </si>
-  <si>
-    <t>CSC</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
-    <t>Spring</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
-    <t>MUS</t>
-  </si>
-  <si>
-    <t>Fall</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Alex Hunter</t>
+  </si>
+  <si>
+    <t>Jacob Anderson</t>
+  </si>
+  <si>
+    <t>Mary Handerson</t>
+  </si>
+  <si>
+    <t>Georeg Alan</t>
   </si>
 </sst>
 </file>
@@ -111,8 +102,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,140 +421,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE20FF1D-4C3E-4B08-BA91-4D7960B91FA1}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1111</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2222</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3333</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4444</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1111</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>191</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>2021</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2222</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>191</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>2021</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1111</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>290</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4">
-        <v>2019</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3333</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>191</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>2021</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4444</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>191</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6">
-        <v>2021</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>